<commit_message>
Version.6 중요도 A, B 일부 완료
</commit_message>
<xml_diff>
--- a/기획+QA.xlsx
+++ b/기획+QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\little Hong\source\repos\PrimerPasoRPG\PrimerPasoRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79367DDD-D415-497D-BB86-33121C64EDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFA1E4F-E5B2-4D08-AE1E-17B8E0E70818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="192">
   <si>
     <t>공격하기</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -598,10 +598,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>현재는 이름 입력 후 직업 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>맵(전투)</t>
   </si>
   <si>
@@ -771,6 +767,14 @@
   </si>
   <si>
     <t>현재는 뒤로가기 제외 모두 1로 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재는 이름 입력 후 화면 초기화 -&gt;직업 선택</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1172,7 +1176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1376,7 +1380,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2055,7 +2058,7 @@
         <v>73</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="64"/>
     </row>
@@ -2067,7 +2070,7 @@
         <v>77</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="64"/>
     </row>
@@ -2079,7 +2082,7 @@
         <v>78</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="64"/>
     </row>
@@ -2123,28 +2126,28 @@
         <v>11</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>154</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="J1" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="K1" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="59" t="s">
         <v>177</v>
-      </c>
-      <c r="L1" s="59" t="s">
-        <v>178</v>
       </c>
       <c r="M1" s="61" t="s">
         <v>13</v>
@@ -2158,7 +2161,7 @@
         <v>74</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="15">
         <v>10</v>
@@ -2204,7 +2207,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" s="15">
         <v>50</v>
@@ -2250,7 +2253,7 @@
         <v>76</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="15">
         <v>150</v>
@@ -4455,10 +4458,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B03DAE-7C2C-40BD-A7FB-06E7A03B2CEF}">
-  <dimension ref="A1:M128"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -4488,7 +4491,7 @@
         <v>87</v>
       </c>
       <c r="G1" s="67" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="H1" s="72"/>
       <c r="I1" s="71"/>
@@ -4526,7 +4529,7 @@
         <v>113</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -4541,7 +4544,7 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G4" s="70" t="s">
         <v>114</v>
@@ -4550,7 +4553,7 @@
         <v>79</v>
       </c>
       <c r="I4" s="67" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M4" s="51"/>
     </row>
@@ -4565,7 +4568,7 @@
         <v>93</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G5" s="70" t="s">
         <v>114</v>
@@ -4574,7 +4577,7 @@
         <v>79</v>
       </c>
       <c r="I5" s="67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M5" s="51"/>
     </row>
@@ -4590,7 +4593,7 @@
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G6" s="70" t="s">
         <v>114</v>
@@ -4599,7 +4602,7 @@
         <v>79</v>
       </c>
       <c r="I6" s="67" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M6" s="51"/>
     </row>
@@ -4614,7 +4617,7 @@
         <v>95</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G7" s="70" t="s">
         <v>114</v>
@@ -4623,7 +4626,7 @@
         <v>79</v>
       </c>
       <c r="I7" s="67" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M7" s="51"/>
     </row>
@@ -4639,7 +4642,7 @@
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G8" s="70" t="s">
         <v>114</v>
@@ -4648,7 +4651,7 @@
         <v>79</v>
       </c>
       <c r="I8" s="67" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M8" s="51"/>
     </row>
@@ -4660,10 +4663,10 @@
         <v>132</v>
       </c>
       <c r="D9" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9" s="39" t="s">
         <v>179</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>180</v>
       </c>
       <c r="G9" s="70" t="s">
         <v>143</v>
@@ -4672,7 +4675,7 @@
         <v>79</v>
       </c>
       <c r="I9" s="67" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M9" s="51"/>
     </row>
@@ -4773,7 +4776,7 @@
         <v>112</v>
       </c>
       <c r="F15" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G15" s="70" t="s">
         <v>118</v>
@@ -4782,7 +4785,7 @@
         <v>79</v>
       </c>
       <c r="I15" s="67" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M15" s="51"/>
     </row>
@@ -5183,15 +5186,17 @@
         <v>145</v>
       </c>
       <c r="F36" s="39" t="s">
-        <v>46</v>
+        <v>179</v>
       </c>
       <c r="G36" s="70" t="s">
-        <v>146</v>
+        <v>191</v>
       </c>
       <c r="H36" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="39"/>
+      <c r="I36" s="67" t="s">
+        <v>190</v>
+      </c>
       <c r="M36" s="53"/>
     </row>
     <row r="37" spans="2:13">
@@ -5202,7 +5207,7 @@
         <v>136</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F37" s="39" t="s">
         <v>46</v>
@@ -5215,19 +5220,19 @@
     </row>
     <row r="38" spans="2:13">
       <c r="B38" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C38" s="39" t="s">
         <v>138</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F38" s="39" t="s">
         <v>46</v>
       </c>
       <c r="G38" s="70" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H38" s="39" t="s">
         <v>79</v>
@@ -5237,13 +5242,13 @@
     </row>
     <row r="39" spans="2:13">
       <c r="B39" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C39" s="39" t="s">
         <v>138</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F39" s="39" t="s">
         <v>46</v>
@@ -5256,16 +5261,16 @@
     </row>
     <row r="40" spans="2:13">
       <c r="B40" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C40" s="39" t="s">
         <v>140</v>
       </c>
       <c r="D40" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="52" t="s">
         <v>158</v>
-      </c>
-      <c r="E40" s="52" t="s">
-        <v>159</v>
       </c>
       <c r="F40" s="39" t="s">
         <v>46</v>
@@ -5278,7 +5283,7 @@
     </row>
     <row r="41" spans="2:13">
       <c r="E41" s="52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F41" s="39" t="s">
         <v>46</v>
@@ -5296,16 +5301,16 @@
         <v>140</v>
       </c>
       <c r="D42" s="52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E42" s="52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F42" s="39" t="s">
         <v>47</v>
       </c>
       <c r="G42" s="70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H42" s="39" t="s">
         <v>79</v>
@@ -5314,13 +5319,13 @@
     </row>
     <row r="43" spans="2:13">
       <c r="E43" s="52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F43" s="39" t="s">
         <v>46</v>
       </c>
       <c r="G43" s="70" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H43" s="39" t="s">
         <v>79</v>
@@ -5335,7 +5340,7 @@
         <v>140</v>
       </c>
       <c r="D44" s="52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F44" s="39" t="s">
         <v>46</v>
@@ -5353,13 +5358,13 @@
         <v>140</v>
       </c>
       <c r="D45" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="F45" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" s="70" t="s">
         <v>170</v>
-      </c>
-      <c r="F45" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="G45" s="70" t="s">
-        <v>171</v>
       </c>
       <c r="H45" s="39" t="s">
         <v>79</v>
@@ -5367,29 +5372,43 @@
       <c r="I45" s="39"/>
     </row>
     <row r="46" spans="2:13">
+      <c r="B46" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" s="52" t="s">
+        <v>171</v>
+      </c>
       <c r="F46" s="39" t="s">
-        <v>46</v>
+        <v>179</v>
+      </c>
+      <c r="G46" s="70" t="s">
+        <v>172</v>
       </c>
       <c r="H46" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="I46" s="39"/>
-    </row>
-    <row r="47" spans="2:13">
+      <c r="I46" s="67" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" ht="34.799999999999997">
       <c r="B47" s="39" t="s">
-        <v>55</v>
+        <v>173</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D47" s="52" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F47" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G47" s="70" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H47" s="39" t="s">
         <v>79</v>
@@ -5398,131 +5417,118 @@
     </row>
     <row r="48" spans="2:13" ht="34.799999999999997">
       <c r="B48" s="39" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="C48" s="39" t="s">
         <v>138</v>
       </c>
       <c r="D48" s="52" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="F48" s="39" t="s">
         <v>46</v>
       </c>
       <c r="G48" s="70" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="H48" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="I48" s="39"/>
-    </row>
-    <row r="49" spans="2:8" ht="34.799999999999997">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9">
       <c r="B49" s="39" t="s">
-        <v>84</v>
+        <v>187</v>
       </c>
       <c r="C49" s="39" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D49" s="52" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F49" s="39" t="s">
-        <v>46</v>
+        <v>179</v>
       </c>
       <c r="G49" s="70" t="s">
-        <v>187</v>
-      </c>
-      <c r="H49" s="39" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="C50" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="D50" s="52" t="s">
         <v>189</v>
       </c>
+      <c r="H49" s="67" t="s">
+        <v>184</v>
+      </c>
+      <c r="I49" s="67" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9">
       <c r="F50" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="G50" s="70" t="s">
-        <v>190</v>
-      </c>
-      <c r="H50" s="67" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8">
+    </row>
+    <row r="51" spans="2:9">
       <c r="F51" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="2:8">
+    <row r="52" spans="2:9">
       <c r="F52" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="2:8">
+    <row r="53" spans="2:9">
       <c r="F53" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="2:8">
+    <row r="54" spans="2:9">
       <c r="F54" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="2:8">
+    <row r="55" spans="2:9">
       <c r="F55" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="2:8">
+    <row r="56" spans="2:9">
       <c r="F56" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="2:8">
+    <row r="57" spans="2:9">
       <c r="F57" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="2:8">
+    <row r="58" spans="2:9">
       <c r="F58" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:8">
+    <row r="59" spans="2:9">
       <c r="F59" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="2:8">
+    <row r="60" spans="2:9">
       <c r="F60" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="2:8">
+    <row r="61" spans="2:9">
       <c r="F61" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="2:8">
+    <row r="62" spans="2:9">
       <c r="F62" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="2:8">
+    <row r="63" spans="2:9">
       <c r="F63" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="2:8">
+    <row r="64" spans="2:9">
       <c r="F64" s="39" t="s">
         <v>46</v>
       </c>
@@ -5839,11 +5845,6 @@
     </row>
     <row r="127" spans="6:6">
       <c r="F127" s="39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="128" spans="6:6">
-      <c r="F128" s="39" t="s">
         <v>46</v>
       </c>
     </row>
@@ -5867,7 +5868,7 @@
       <formula>NOT(ISERROR(SEARCH("Pass",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C128">
+  <conditionalFormatting sqref="C4:C127">
     <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",C4)))</formula>
     </cfRule>
@@ -5965,7 +5966,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>137</v>
@@ -6016,7 +6017,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="8" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>